<commit_message>
ajouts pour ESPLE, SecSelfAdapt et SmellReprod
</commit_message>
<xml_diff>
--- a/Datasets/_Datasets Sent/Datasets_overview.xlsx
+++ b/Datasets/_Datasets Sent/Datasets_overview.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="ESM_2" sheetId="1" state="visible" r:id="rId3"/>
@@ -16,13 +16,14 @@
     <sheet name="Behave" sheetId="6" state="visible" r:id="rId8"/>
     <sheet name="TrustSE" sheetId="7" state="visible" r:id="rId9"/>
     <sheet name="ESPLE" sheetId="8" state="visible" r:id="rId10"/>
-    <sheet name="OODP" sheetId="9" state="visible" r:id="rId11"/>
-    <sheet name="ModelingAssist" sheetId="10" state="visible" r:id="rId12"/>
+    <sheet name="SmellReprod" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="SecSelfAdapt" sheetId="10" state="visible" r:id="rId12"/>
     <sheet name="ModelGuidance" sheetId="11" state="visible" r:id="rId13"/>
-    <sheet name="ArchiML" sheetId="12" state="visible" r:id="rId14"/>
-    <sheet name="CodeClone" sheetId="13" state="visible" r:id="rId15"/>
-    <sheet name="CodeCompr" sheetId="14" state="visible" r:id="rId16"/>
-    <sheet name="SecSelfAdapt" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="OODP" sheetId="12" state="visible" r:id="rId14"/>
+    <sheet name="ModelingAssist" sheetId="13" state="visible" r:id="rId15"/>
+    <sheet name="ArchiML" sheetId="14" state="visible" r:id="rId16"/>
+    <sheet name="CodeClone" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="CodeCompr" sheetId="16" state="visible" r:id="rId18"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="70">
   <si>
     <t xml:space="preserve">Overview</t>
   </si>
@@ -196,6 +197,54 @@
   </si>
   <si>
     <t xml:space="preserve">A Survey on Trust Management [J]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESPLE-filtered-source.tsv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESPLE-screened-source.tsv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available from data source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SmellReprod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SmellReprod[include decision] == Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SmellReprod[Final result] == Accepted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Has a lot of proceedings as articles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proceedings - International Conference on Software Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proceedings - International Computer Software and Applications Conference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACM International Conference Proceeding Series</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICEIS 2017 - Proceedings of the 19th International Conference on Enterprise Information Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International Symposium on Empirical Software Engineering and Measurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESEM 2010 - Proceedings of the 2010 ACM-IEEE International Symposium on Empirical Software Engineering and Measurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge Results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full  text reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full  text reading[last column] = 4</t>
   </si>
 </sst>
 </file>
@@ -205,7 +254,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +292,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -252,7 +308,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -260,8 +316,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -285,8 +348,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -303,19 +369,88 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Pivot Table Category" xfId="20"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -613,8 +748,8 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -645,20 +780,68 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="1" t="n">
+        <v>1433</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <f aca="false">B2-D2</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1433</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B3" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <f aca="false">B3-D3</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <f aca="false">B5-D5</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1056,6 +1239,81 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="12.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.45"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1656,7 +1914,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1848,7 +2106,7 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1886,7 +2144,7 @@
       <c r="C2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>553</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1903,7 +2161,7 @@
       <c r="C3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>112</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1920,7 +2178,7 @@
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1928,13 +2186,13 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1990,7 +2248,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2021,20 +2279,67 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="1" t="n">
+        <v>963</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <f aca="false">B2-D2</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>963</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B3" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <f aca="false">B3-D3</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2062,20 +2367,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="12.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.45"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2088,46 +2388,262 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="n">
+        <v>1733</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <f aca="false">B2-D2</f>
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1714</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <f aca="false">B3-D3</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <f aca="false">B5-D5</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C8" s="1"/>
       <c r="E8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added info for OODP
</commit_message>
<xml_diff>
--- a/Datasets/_Datasets Sent/Datasets_overview.xlsx
+++ b/Datasets/_Datasets Sent/Datasets_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udemontreal-my.sharepoint.com/personal/guillaume_genois_umontreal_ca/Documents/Projet Curation des métadonnées/Datasets/_Datasets Sent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="11_959E167E478734F10FDD2A89CBA50D2011D30D8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59F8B926-B99F-4E9C-9BEB-79929D9D7142}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="11_959E167E478734F10FDD2A89CBA50D2011D30D8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0ED3A91-F5F2-4B61-B411-8E233A708395}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="153">
   <si>
     <t>Overview</t>
   </si>
@@ -498,6 +498,18 @@
   </si>
   <si>
     <t>Public transport. Service interface for real-time information relating to public transport operations. Context and framework</t>
+  </si>
+  <si>
+    <t>144 supposed according to article, but not in source excel</t>
+  </si>
+  <si>
+    <t>query results</t>
+  </si>
+  <si>
+    <t>Included</t>
+  </si>
+  <si>
+    <t>The following articles were not found, but some metadata were already in data source such as the abstract, so they were kept.</t>
   </si>
 </sst>
 </file>
@@ -1141,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1173,21 +1185,71 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2">
+        <v>685</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>685</v>
+      </c>
+      <c r="E2" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
+      <c r="B5">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -1611,7 +1673,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ajout ModelGuidance et OODP
</commit_message>
<xml_diff>
--- a/Datasets/_Datasets Sent/Datasets_overview.xlsx
+++ b/Datasets/_Datasets Sent/Datasets_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udemontreal-my.sharepoint.com/personal/guillaume_genois_umontreal_ca/Documents/Projet Curation des métadonnées/Datasets/_Datasets Sent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="11_959E167E478734F10FDD2A89CBA50D2011D30D8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{168AD1F0-EB08-4DD3-80B1-C077C30E8738}"/>
+  <xr:revisionPtr revIDLastSave="299" documentId="11_959E167E478734F10FDD2A89CBA50D2011D30D8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EAE175D-A788-49E6-AD73-6037F765D8FB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-26550" yWindow="2250" windowWidth="21600" windowHeight="11295" tabRatio="500" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ESM_2" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,13 @@
     <sheet name="SecSelfAdapt" sheetId="10" r:id="rId10"/>
     <sheet name="ModelGuidance" sheetId="11" r:id="rId11"/>
     <sheet name="OODP" sheetId="12" r:id="rId12"/>
-    <sheet name="ModelingAssist" sheetId="13" r:id="rId13"/>
-    <sheet name="ArchiML" sheetId="14" r:id="rId14"/>
-    <sheet name="CodeClone" sheetId="15" r:id="rId15"/>
-    <sheet name="CodeCompr" sheetId="16" r:id="rId16"/>
+    <sheet name="ArchiML" sheetId="14" r:id="rId13"/>
+    <sheet name="CodeCompr" sheetId="16" r:id="rId14"/>
+    <sheet name="ModelingAssist" sheetId="13" r:id="rId15"/>
+    <sheet name="CodeClone" sheetId="15" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="243">
   <si>
     <t>Overview</t>
   </si>
@@ -296,9 +297,6 @@
     <t>Aspect oriented programming paradigm</t>
   </si>
   <si>
-    <t>À vérifier</t>
-  </si>
-  <si>
     <t>Choosing a framework in open source development</t>
   </si>
   <si>
@@ -509,9 +507,6 @@
     <t>Included</t>
   </si>
   <si>
-    <t>The following articles were not found, but some metadata were already in data source such as the abstract, so they were kept.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Tomi; Soininen</t>
   </si>
   <si>
@@ -606,6 +601,186 @@
   </si>
   <si>
     <t>From the Journalsâ€¦</t>
+  </si>
+  <si>
+    <t>Code-First Model-Driven Engineering: On the Agile Adoption of MDE Tooling</t>
+  </si>
+  <si>
+    <t>Progress and Quality Modeling of Requirements Analysis Based on Chaos</t>
+  </si>
+  <si>
+    <t>Using Responsibilities for Early Identification of Hot Spots Reused in Frameworks Modeling</t>
+  </si>
+  <si>
+    <t>Ontology-based feature modeling: An empirical study in changing scenarios</t>
+  </si>
+  <si>
+    <t>Object-oriented modeling method for algebraic specifications in CafeOBJ</t>
+  </si>
+  <si>
+    <t>Features of integrated model-based co-modelling and co-simulation technology</t>
+  </si>
+  <si>
+    <t>Modeling and managing the variability of Web service-based systems</t>
+  </si>
+  <si>
+    <t>Dynamic Non-functional Requirements Based Model-Driven Agent Development</t>
+  </si>
+  <si>
+    <t>A UML-based object-oriented framework development methodology</t>
+  </si>
+  <si>
+    <t>A Model Driven Method to Design and Analyze Secure Architectures of Systems-of-Systems</t>
+  </si>
+  <si>
+    <t>Integrating organizational requirements and object oriented modeling</t>
+  </si>
+  <si>
+    <t>MODELLING STYLES AND THEIR SUPPORT IN THE CASM ENVIRONMENT.</t>
+  </si>
+  <si>
+    <t>A modeling methodology to facilitate safety-oriented architecture design of industrial avionics software</t>
+  </si>
+  <si>
+    <t>Modeling Human Behavior for Software Engineering Simulation Games</t>
+  </si>
+  <si>
+    <t>Security patterns modeling and formalization for pattern-based development of secure software systems</t>
+  </si>
+  <si>
+    <t>Extending BPMN with submit/response-style user interaction modeling</t>
+  </si>
+  <si>
+    <t>Integrating organizational requirements and object oriented modelling</t>
+  </si>
+  <si>
+    <t>UML-B: Formal Modeling and Design Aided by UML</t>
+  </si>
+  <si>
+    <t>Implication of different learning styles on the modeling of object-oriented systems</t>
+  </si>
+  <si>
+    <t>Middleware-Induced Architectural Style Modelling for Architecture Exploration</t>
+  </si>
+  <si>
+    <t>Modeling and reasoning about design alternatives of software as a service architectures</t>
+  </si>
+  <si>
+    <t>Modeling of Architectures with UML Panel</t>
+  </si>
+  <si>
+    <t>An integrated role-based approach for modeling, designing and implementing multi-agent systems</t>
+  </si>
+  <si>
+    <t>Extending the UML Statecharts Notation to Model Security Aspects</t>
+  </si>
+  <si>
+    <t>Model-driven secure development lifecycle</t>
+  </si>
+  <si>
+    <t>Model driven software development: An overview</t>
+  </si>
+  <si>
+    <t>Towards a Model-Integrated Runtime Monitoring Infrastructure for Cyber-Physical Systems</t>
+  </si>
+  <si>
+    <t>Automatic generation of UML profile graphical editors for Papyrus</t>
+  </si>
+  <si>
+    <t>Model-based performance risk analysis</t>
+  </si>
+  <si>
+    <t>Model-based performance analysis of software architectures under uncertainty</t>
+  </si>
+  <si>
+    <t>Model-based verification of safety contracts</t>
+  </si>
+  <si>
+    <t>Generating model with uncertainty by means of JTL</t>
+  </si>
+  <si>
+    <t>Identifying and Managing Complex Modules in Executable Software Design Models-Empirical Assessment of a Large Telecom Software Product</t>
+  </si>
+  <si>
+    <t>Checking architectural and implementation constraints for domain-specific component frameworks using models</t>
+  </si>
+  <si>
+    <t>Model-driven development of condition monitoring software</t>
+  </si>
+  <si>
+    <t>step4analysis</t>
+  </si>
+  <si>
+    <t>step2abstract_search1 + step2abstract_search2</t>
+  </si>
+  <si>
+    <t>step3fulltext_search1 + step3fulltext_search3</t>
+  </si>
+  <si>
+    <t>duplicate</t>
+  </si>
+  <si>
+    <t>duplicate x2</t>
+  </si>
+  <si>
+    <t>not available</t>
+  </si>
+  <si>
+    <t>duplicate of articles across search 1 and 2</t>
+  </si>
+  <si>
+    <t>duplicate of "An Object-Oriented Modeling Method for Algebraic Specifications in CafeOBJ"</t>
+  </si>
+  <si>
+    <t>duplicate of "Integrating organizational requirements and object oriented modeling"</t>
+  </si>
+  <si>
+    <t>duplicate of "Modelling Styles and Their Support in the CASM Environment"</t>
+  </si>
+  <si>
+    <t>duplicate of "The implication of different learning styles on the modeling of object-oriented systems"</t>
+  </si>
+  <si>
+    <t>joined to the initial selection, because some were not present in the re-run of the query</t>
+  </si>
+  <si>
+    <t>An incremental project plan: introducing cleanroom method and object-oriented development method</t>
+  </si>
+  <si>
+    <t>duplicate of "Incremental project plan: Introducing cleanroom method and object-oriented development method"</t>
+  </si>
+  <si>
+    <t>An object-based information retrieval model: toward the structural construction of thesauri</t>
+  </si>
+  <si>
+    <t>duplicate of "Object-based information retrieval model: Toward the structural construction of thesauri"</t>
+  </si>
+  <si>
+    <t>Patterns of agent interaction scenarios as use case maps</t>
+  </si>
+  <si>
+    <t>duplicate of "Pattern oriented service development for coarse-grained service reuse"</t>
+  </si>
+  <si>
+    <t>The numbers don't match the paper because the author re-ran the query to send me the list of all papers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The following articles were not found, but some metadata were already in data source such as the abstract, so they were kept. </t>
+  </si>
+  <si>
+    <t>All papers</t>
+  </si>
+  <si>
+    <t>screening</t>
+  </si>
+  <si>
+    <t>Selection Criteria</t>
+  </si>
+  <si>
+    <t>Selection Criteria[Selected==True]</t>
+  </si>
+  <si>
+    <t>Final Paper</t>
   </si>
 </sst>
 </file>
@@ -684,12 +859,15 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1075,14 +1253,14 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1113,7 +1291,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1127,7 +1305,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1135,7 +1313,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1149,12 +1327,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1163,7 +1341,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1182,14 +1360,14 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1206,7 +1384,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1224,7 +1402,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1242,7 +1420,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1256,7 +1434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1274,7 +1452,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1291,20 +1469,21 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1321,27 +1500,85 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <f>1009+768</f>
+        <v>1777</v>
+      </c>
+      <c r="C2">
+        <f>B2-D2</f>
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>1741</v>
+      </c>
+      <c r="E2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <f>111+110</f>
+        <v>221</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C5" si="0">B3-D3</f>
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>220</v>
+      </c>
+      <c r="E3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1350,28 +1587,308 @@
       </c>
       <c r="E8" s="1"/>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B18" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B21" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B23" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B25" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B26" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B27" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B28" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B30" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B31" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B32" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B33" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B34" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B36" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B37" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B38" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B39" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>187</v>
+      </c>
+      <c r="B40" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>199</v>
+      </c>
+      <c r="B41" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>194</v>
+      </c>
+      <c r="B42" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" t="s">
+        <v>228</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1388,24 +1905,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>685</v>
+        <v>713</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <f>B2-D2</f>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>685</v>
+        <v>710</v>
       </c>
       <c r="E2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1418,11 +1936,11 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1436,7 +1954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1450,15 +1968,18 @@
         <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1467,415 +1988,441 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>76</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>78</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>80</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="B23" t="s">
         <v>83</v>
       </c>
-      <c r="B19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>92</v>
-      </c>
-      <c r="B23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>93</v>
       </c>
       <c r="B24" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>95</v>
       </c>
-      <c r="B25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="B30" t="s">
         <v>96</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>98</v>
       </c>
-      <c r="B27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>99</v>
       </c>
-      <c r="B28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" t="s">
         <v>100</v>
       </c>
-      <c r="B29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>102</v>
       </c>
-      <c r="B30" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="B35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>103</v>
       </c>
-      <c r="B31" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="B36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" t="s">
         <v>104</v>
       </c>
-      <c r="B32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>106</v>
       </c>
-      <c r="B33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" t="s">
         <v>107</v>
       </c>
-      <c r="B34" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" t="s">
         <v>109</v>
       </c>
-      <c r="B35" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>111</v>
       </c>
-      <c r="B36" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>112</v>
       </c>
-      <c r="B37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>113</v>
       </c>
-      <c r="B38" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="B43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>114</v>
       </c>
-      <c r="B39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>116</v>
+      </c>
+      <c r="B45" t="s">
         <v>115</v>
       </c>
-      <c r="B40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>117</v>
       </c>
-      <c r="B41" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="B46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>118</v>
       </c>
-      <c r="B42" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="B47" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" t="s">
         <v>119</v>
       </c>
-      <c r="B43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>121</v>
       </c>
-      <c r="B44" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="B49" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>122</v>
       </c>
-      <c r="B45" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="B50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" t="s">
         <v>123</v>
       </c>
-      <c r="B46" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>126</v>
+      </c>
+      <c r="B52" t="s">
         <v>125</v>
       </c>
-      <c r="B47" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>127</v>
       </c>
-      <c r="B48" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="B53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" t="s">
         <v>128</v>
       </c>
-      <c r="B49" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>130</v>
       </c>
-      <c r="B50" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="B55" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>131</v>
       </c>
-      <c r="B51" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="B56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" t="s">
         <v>132</v>
       </c>
-      <c r="B52" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>135</v>
+      </c>
+      <c r="B58" t="s">
         <v>134</v>
       </c>
-      <c r="B53" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>136</v>
       </c>
-      <c r="B54" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>137</v>
       </c>
-      <c r="B55" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="B60" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>138</v>
       </c>
-      <c r="B56" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+      <c r="B61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>139</v>
       </c>
-      <c r="B57" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+      <c r="B62" t="s">
         <v>140</v>
       </c>
-      <c r="B58" t="s">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+      <c r="B63" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>142</v>
       </c>
-      <c r="B59" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+      <c r="B64" t="s">
         <v>143</v>
       </c>
-      <c r="B60" t="s">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+      <c r="B65" t="s">
         <v>145</v>
       </c>
-      <c r="B61" t="s">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>147</v>
+      </c>
+      <c r="B66" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>148</v>
-      </c>
-      <c r="B62" t="s">
-        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1885,6 +2432,490 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>2766</v>
+      </c>
+      <c r="C2">
+        <f>B2-D2</f>
+        <v>2766</v>
+      </c>
+      <c r="E2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C5" si="0">B3-D3</f>
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>165</v>
+      </c>
+      <c r="B22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>168</v>
+      </c>
+      <c r="B25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>172</v>
+      </c>
+      <c r="B29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>174</v>
+      </c>
+      <c r="B31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>177</v>
+      </c>
+      <c r="B34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>178</v>
+      </c>
+      <c r="B35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>179</v>
+      </c>
+      <c r="B36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>181</v>
+      </c>
+      <c r="B38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>3999</v>
+      </c>
+      <c r="C2">
+        <f>B2-D2</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>3999</v>
+      </c>
+      <c r="E2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>550</v>
+      </c>
+      <c r="C3">
+        <f>B3-D3</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>550</v>
+      </c>
+      <c r="E3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -1892,14 +2923,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1916,27 +2947,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1951,355 +2982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:E39"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>153</v>
-      </c>
-      <c r="B9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>156</v>
-      </c>
-      <c r="B11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>157</v>
-      </c>
-      <c r="B12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>160</v>
-      </c>
-      <c r="B15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>162</v>
-      </c>
-      <c r="B17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>163</v>
-      </c>
-      <c r="B18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>164</v>
-      </c>
-      <c r="B19" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>165</v>
-      </c>
-      <c r="B20" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>166</v>
-      </c>
-      <c r="B21" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>167</v>
-      </c>
-      <c r="B22" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>168</v>
-      </c>
-      <c r="B23" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>169</v>
-      </c>
-      <c r="B24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>170</v>
-      </c>
-      <c r="B25" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>171</v>
-      </c>
-      <c r="B26" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>172</v>
-      </c>
-      <c r="B27" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>173</v>
-      </c>
-      <c r="B28" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>174</v>
-      </c>
-      <c r="B29" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>175</v>
-      </c>
-      <c r="B30" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>176</v>
-      </c>
-      <c r="B31" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>177</v>
-      </c>
-      <c r="B32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>178</v>
-      </c>
-      <c r="B33" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>179</v>
-      </c>
-      <c r="B34" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>180</v>
-      </c>
-      <c r="B35" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>181</v>
-      </c>
-      <c r="B36" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>182</v>
-      </c>
-      <c r="B37" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>183</v>
-      </c>
-      <c r="B38" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>184</v>
-      </c>
-      <c r="B39" t="s">
-        <v>154</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="8" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="6" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="4" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -2307,14 +2990,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2331,94 +3014,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -2441,14 +3057,14 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2465,7 +3081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2479,7 +3095,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2493,7 +3109,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2507,7 +3123,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2521,7 +3137,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2535,7 +3151,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -2544,7 +3160,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2563,14 +3179,14 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2587,7 +3203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2603,7 +3219,7 @@
         <v>3489</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2621,7 +3237,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2639,7 +3255,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2654,7 +3270,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2672,7 +3288,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2687,7 +3303,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2705,7 +3321,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -2727,14 +3343,14 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2751,7 +3367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2767,7 +3383,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2785,7 +3401,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2803,7 +3419,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2818,7 +3434,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2836,7 +3452,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2851,7 +3467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2869,7 +3485,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -2886,20 +3502,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2916,7 +3535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2934,7 +3553,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2952,7 +3571,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2960,7 +3579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2978,7 +3597,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -2998,17 +3617,17 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3025,7 +3644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3033,16 +3652,17 @@
         <v>601</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <f>B2-D2</f>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3050,6 +3670,7 @@
         <v>148</v>
       </c>
       <c r="C3">
+        <f>B3-D3</f>
         <v>4</v>
       </c>
       <c r="D3">
@@ -3059,7 +3680,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3067,7 +3688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3075,7 +3696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -3084,7 +3705,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -3092,7 +3713,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -3100,7 +3721,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -3108,7 +3729,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -3116,7 +3737,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -3124,7 +3745,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -3132,7 +3753,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -3140,7 +3761,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -3148,7 +3769,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -3156,7 +3777,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -3164,7 +3785,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -3186,14 +3807,14 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3210,7 +3831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3227,7 +3848,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3244,7 +3865,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3258,7 +3879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3272,7 +3893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -3281,7 +3902,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -3289,7 +3910,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -3297,7 +3918,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -3319,14 +3940,14 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3343,7 +3964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3361,7 +3982,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3379,7 +4000,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3393,7 +4014,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3410,7 +4031,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -3430,12 +4051,12 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3452,7 +4073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3470,7 +4091,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3488,7 +4109,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3502,7 +4123,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3520,12 +4141,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -3534,7 +4155,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -3542,7 +4163,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -3550,7 +4171,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>63</v>
       </c>
@@ -3558,7 +4179,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>63</v>
       </c>
@@ -3566,7 +4187,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>63</v>
       </c>
@@ -3574,7 +4195,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>63</v>
       </c>
@@ -3582,7 +4203,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>63</v>
       </c>
@@ -3590,7 +4211,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
@@ -3598,7 +4219,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
@@ -3606,7 +4227,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
@@ -3614,7 +4235,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
@@ -3622,7 +4243,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
@@ -3630,7 +4251,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>36</v>
       </c>
@@ -3638,7 +4259,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -3646,7 +4267,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -3654,7 +4275,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -3662,7 +4283,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -3670,7 +4291,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -3678,7 +4299,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>66</v>
       </c>

</xml_diff>